<commit_message>
Added Cross Browser Testing
</commit_message>
<xml_diff>
--- a/src/test/resources/runmanager/TestData.xlsx
+++ b/src/test/resources/runmanager/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t xml:space="preserve">MethodName</t>
   </si>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
+    <t xml:space="preserve">Browser</t>
+  </si>
+  <si>
     <t xml:space="preserve">userName</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
     <t xml:space="preserve">fname</t>
   </si>
   <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
@@ -77,7 +83,7 @@
     <t xml:space="preserve">Peppa</t>
   </si>
   <si>
-    <t xml:space="preserve">admin124</t>
+    <t xml:space="preserve">firefox</t>
   </si>
   <si>
     <t xml:space="preserve">Susi</t>
@@ -188,11 +194,11 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.99"/>
@@ -268,19 +274,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="9.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,6 +305,9 @@
       <c r="E1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -308,13 +317,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,13 +337,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>19</v>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,13 +357,16 @@
         <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,13 +377,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -376,13 +397,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom Annotation To add Author & Category
</commit_message>
<xml_diff>
--- a/src/test/resources/runmanager/TestData.xlsx
+++ b/src/test/resources/runmanager/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t xml:space="preserve">MethodName</t>
   </si>
@@ -44,21 +44,24 @@
     <t xml:space="preserve">This test to Login and Logout Functionality</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing an another method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verifyBooksPageTitle</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing an another method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">Browser</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
     <t xml:space="preserve">fname</t>
   </si>
   <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
     <t xml:space="preserve">chrome</t>
   </si>
   <si>
@@ -83,6 +89,9 @@
     <t xml:space="preserve">Peppa</t>
   </si>
   <si>
+    <t xml:space="preserve">'</t>
+  </si>
+  <si>
     <t xml:space="preserve">firefox</t>
   </si>
   <si>
@@ -92,10 +101,10 @@
     <t xml:space="preserve">Emly</t>
   </si>
   <si>
-    <t xml:space="preserve">'</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book</t>
   </si>
 </sst>
 </file>
@@ -192,13 +201,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.99"/>
@@ -249,12 +258,29 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -274,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
@@ -297,16 +323,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,16 +346,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,16 +369,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,18 +389,21 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -377,16 +415,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,19 +435,45 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>24</v>
+      <c r="D7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docker Compose with Sel Grid
</commit_message>
<xml_diff>
--- a/src/test/resources/runmanager/TestData.xlsx
+++ b/src/test/resources/runmanager/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t xml:space="preserve">MethodName</t>
   </si>
@@ -203,11 +203,11 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.99"/>
@@ -300,13 +300,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
@@ -476,6 +476,29 @@
         <v>27</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Min Price Rows Page Test
</commit_message>
<xml_diff>
--- a/src/test/resources/runmanager/TestData.xlsx
+++ b/src/test/resources/runmanager/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
   <si>
     <t xml:space="preserve">MethodName</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t xml:space="preserve">To Test if any broken links are there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testMinRowSelection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Test the Min Row is Selected</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -219,13 +225,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.99"/>
@@ -344,12 +350,29 @@
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>8</v>
       </c>
     </row>
@@ -369,13 +392,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
@@ -392,19 +415,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,19 +438,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,19 +461,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -461,19 +484,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,19 +507,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,19 +530,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,19 +553,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,19 +576,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,19 +599,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,19 +622,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -619,22 +642,45 @@
         <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>28</v>
+      <c r="B12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>